<commit_message>
add epl column to sup table
</commit_message>
<xml_diff>
--- a/sup_table.xlsx
+++ b/sup_table.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -407,6 +407,11 @@
           <t>error_max_abs</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>epl</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -452,6 +457,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -497,6 +507,11 @@
           <t>1020</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.031</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -542,6 +557,11 @@
           <t>688</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -587,6 +607,11 @@
           <t>348</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -632,6 +657,11 @@
           <t>431</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.129</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -677,6 +707,11 @@
           <t>1221</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.288</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -722,6 +757,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -767,6 +807,11 @@
           <t>656</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.042</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -812,6 +857,11 @@
           <t>369</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.046</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -857,6 +907,11 @@
           <t>220</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.085</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -902,6 +957,11 @@
           <t>298</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.168</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -947,6 +1007,11 @@
           <t>670</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.393</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -992,6 +1057,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1037,6 +1107,11 @@
           <t>395</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.047</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1082,6 +1157,11 @@
           <t>285</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.066</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1127,6 +1207,11 @@
           <t>117</t>
         </is>
       </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.107</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1172,6 +1257,11 @@
           <t>160</t>
         </is>
       </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.153</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1217,6 +1307,11 @@
           <t>421</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0.490</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1262,6 +1357,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1307,6 +1407,11 @@
           <t>397</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.081</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1352,6 +1457,11 @@
           <t>344</t>
         </is>
       </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.085</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1397,6 +1507,11 @@
           <t>91</t>
         </is>
       </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.141</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1442,6 +1557,11 @@
           <t>165</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0.166</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1487,6 +1607,11 @@
           <t>295</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>0.488</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1532,6 +1657,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1577,6 +1707,11 @@
           <t>210</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>0.130</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1622,6 +1757,11 @@
           <t>115</t>
         </is>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0.157</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1667,6 +1807,11 @@
           <t>37</t>
         </is>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>0.270</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1712,6 +1857,11 @@
           <t>73</t>
         </is>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0.262</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1757,6 +1907,11 @@
           <t>149</t>
         </is>
       </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>0.715</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1802,6 +1957,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1847,6 +2007,11 @@
           <t>88</t>
         </is>
       </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>0.275</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1892,6 +2057,11 @@
           <t>57</t>
         </is>
       </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>0.304</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1937,6 +2107,11 @@
           <t>23</t>
         </is>
       </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>0.531</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1982,6 +2157,11 @@
           <t>46</t>
         </is>
       </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>0.460</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2027,6 +2207,11 @@
           <t>101</t>
         </is>
       </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>0.450</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2072,6 +2257,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2117,6 +2307,11 @@
           <t>66</t>
         </is>
       </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>0.426</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2162,6 +2357,11 @@
           <t>45</t>
         </is>
       </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>0.427</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2207,6 +2407,11 @@
           <t>19</t>
         </is>
       </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0.716</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2252,6 +2457,11 @@
           <t>25</t>
         </is>
       </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>0.659</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2297,6 +2507,11 @@
           <t>63</t>
         </is>
       </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>0.662</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2342,6 +2557,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2387,6 +2607,11 @@
           <t>185</t>
         </is>
       </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>0.758</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2432,6 +2657,11 @@
           <t>39</t>
         </is>
       </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0.524</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2477,6 +2707,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>0.818</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2522,6 +2757,11 @@
           <t>24</t>
         </is>
       </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>0.819</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2565,6 +2805,11 @@
       <c r="I49" t="inlineStr">
         <is>
           <t>43</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>0.850</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ENH: re-run all analyses
and get the result generation notebook into the repo
</commit_message>
<xml_diff>
--- a/sup_table.xlsx
+++ b/sup_table.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.031</t>
+          <t>0.014</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.024</t>
+          <t>0.017</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.067</t>
+          <t>0.119</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.129</t>
+          <t>0.126</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.288</t>
+          <t>0.139</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.042</t>
+          <t>0.035</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.046</t>
+          <t>0.033</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.085</t>
+          <t>0.104</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0.168</t>
+          <t>0.165</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0.393</t>
+          <t>0.200</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.038</t>
         </is>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.066</t>
+          <t>0.046</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.107</t>
+          <t>0.166</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.153</t>
+          <t>0.150</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0.490</t>
+          <t>0.225</t>
         </is>
       </c>
     </row>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.081</t>
+          <t>0.048</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.085</t>
+          <t>0.064</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0.141</t>
+          <t>0.166</t>
         </is>
       </c>
     </row>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>0.166</t>
+          <t>0.164</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0.488</t>
+          <t>0.241</t>
         </is>
       </c>
     </row>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0.130</t>
+          <t>0.094</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>0.157</t>
+          <t>0.116</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>0.270</t>
+          <t>0.300</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>0.262</t>
+          <t>0.253</t>
         </is>
       </c>
     </row>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>0.715</t>
+          <t>0.280</t>
         </is>
       </c>
     </row>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>0.275</t>
+          <t>0.169</t>
         </is>
       </c>
     </row>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>0.304</t>
+          <t>0.219</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>0.531</t>
+          <t>0.453</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>0.460</t>
+          <t>0.445</t>
         </is>
       </c>
     </row>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0.426</t>
+          <t>0.225</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>0.427</t>
+          <t>0.299</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>0.716</t>
+          <t>0.541</t>
         </is>
       </c>
     </row>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>0.659</t>
+          <t>0.626</t>
         </is>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>0.662</t>
+          <t>0.652</t>
         </is>
       </c>
     </row>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>0.758</t>
+          <t>0.318</t>
         </is>
       </c>
     </row>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>0.524</t>
+          <t>0.381</t>
         </is>
       </c>
     </row>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>0.818</t>
+          <t>0.742</t>
         </is>
       </c>
     </row>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>0.819</t>
+          <t>0.722</t>
         </is>
       </c>
     </row>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>0.850</t>
+          <t>0.743</t>
         </is>
       </c>
     </row>

</xml_diff>